<commit_message>
update to add the currency result calculator
</commit_message>
<xml_diff>
--- a/PriceTargetCalculator.xlsx
+++ b/PriceTargetCalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\curr-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EC30DBEA-1ACC-4F39-BABC-FA90BB879BDF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6CD9EAC2-7A23-4C40-AD86-3A85D0DE5A8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{9F132E27-25D6-4B8C-865D-8CBD74D7F44D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Enter Price</t>
   </si>
@@ -37,6 +37,45 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Exit 1 Ratio</t>
+  </si>
+  <si>
+    <t>Exit 1 Price</t>
+  </si>
+  <si>
+    <t>Exit 2 Ratio</t>
+  </si>
+  <si>
+    <t>Exit 2 Price</t>
+  </si>
+  <si>
+    <t>Exit 3 Ratio</t>
+  </si>
+  <si>
+    <t>Exit 3 Price</t>
+  </si>
+  <si>
+    <t>Exit 4 Ratio</t>
+  </si>
+  <si>
+    <t>Exit 4 Price</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Exit2 R</t>
+  </si>
+  <si>
+    <t>Exit1 R</t>
+  </si>
+  <si>
+    <t>Exit3 R</t>
+  </si>
+  <si>
+    <t>Exit4 R</t>
   </si>
 </sst>
 </file>
@@ -400,84 +439,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25EC243-FDFE-4BAD-B77D-6BC7638C2790}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="D1" sqref="D1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <f>$H$3*$E$4 +$H$4*$E$6+$H$5*$E$8+$H$6*E10</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>85.19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.5501</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>B2</f>
+        <v>1.5501</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>E2-E3</f>
+        <v>-3.9999999999995595E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>85.14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.5505</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>B3</f>
+        <v>1.5505</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <f>IF(ISBLANK(E5), 0, (E5-$E$2) / $H$2)</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <f>B2-B3</f>
-        <v>4.9999999999997158E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-3.9999999999995595E-4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <f>IF(ISBLANK(E7), 0, (E7-$E$2) / $H$2)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.2</v>
       </c>
       <c r="B5" s="2">
         <f>IF($A$1=1,$B$2+$B$4*A5,$B$2-A5*$B$4)</f>
-        <v>85.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.54962</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1.5494000000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <f>IF(ISBLANK(E9), 0, (E9-$E$2) / $H$2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B8" si="0">IF($A$1=1,$B$2+$B$4*A6,$B$2-A6*$B$4)</f>
-        <v>85.289999999999992</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.5493000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>0.75</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <f>IF(ISBLANK(E11), 0, (E11-$E$2) / $H$2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>85.389999999999986</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.5485000000000002</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>85.589999999999975</v>
+        <v>1.5469000000000004</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>